<commit_message>
create a visual of Box of Revenue by genre
</commit_message>
<xml_diff>
--- a/Movie_Data_Starter_Project.xlsx
+++ b/Movie_Data_Starter_Project.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\Movie_Data_Pivot_Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795FD225-1F25-4086-BE8C-001CD139760E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC6BC9F-036D-49A0-9A8B-3F723FACBFEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="16" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -8675,7 +8675,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -8690,6 +8693,1076 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Movie_Data_Starter_Project.xlsx]Summary!PivotTable1</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average of Box Office Revenue($)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> by Genre</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$4:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>Action</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Adventure</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Animation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Biography</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Comedy</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Crime</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Documentary</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Drama</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Family</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Fantasy</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Horror</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Musical</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Mystery</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Religious</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Romance</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Sci-Fi</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Thriller</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$4:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>233839500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>308633333.33333331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>276200000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58806666.666666664</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>123442857.14285715</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57669565.217391305</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80990337.078651682</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>270958333.33333331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>244610000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>75646511.627906978</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>130000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>96780000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36914285.714285716</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>53705384.615384616</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>255443571.42857143</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>136937500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-278F-4BD0-883D-834563966A21}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="836405296"/>
+        <c:axId val="815720688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="836405296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="815720688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="815720688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="836405296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBAE152C-4E07-44DC-9660-87626E9F25A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16901,7 +17974,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{03D8EE8E-B7D7-44CF-B947-606DF35C4542}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{03D8EE8E-B7D7-44CF-B947-606DF35C4542}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -17006,10 +18079,21 @@
     <dataField name="Average of Box Office Revenue ($)" fld="13" subtotal="average" baseField="3" baseItem="0" numFmtId="43"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="0">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
+  <chartFormats count="1">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -17322,13 +18406,15 @@
   <dimension ref="A3:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -17485,6 +18571,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
sort the data by 'Average of Box Office Revenue'
</commit_message>
<xml_diff>
--- a/Movie_Data_Starter_Project.xlsx
+++ b/Movie_Data_Starter_Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\Movie_Data_Pivot_Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC6BC9F-036D-49A0-9A8B-3F723FACBFEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A92CE0-54A4-4730-A9A3-C26AC3E6633E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8675,7 +8675,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -8842,55 +8854,55 @@
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>Action</c:v>
+                  <c:v>Religious</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Adventure</c:v>
+                  <c:v>Romance</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Animation</c:v>
+                  <c:v>Crime</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Biography</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Documentary</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Horror</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Drama</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mystery</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Comedy</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Crime</c:v>
+                <c:pt idx="9">
+                  <c:v>Musical</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>Documentary</c:v>
+                <c:pt idx="10">
+                  <c:v>Thriller</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>Drama</c:v>
+                <c:pt idx="11">
+                  <c:v>Action</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
+                  <c:v>Fantasy</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Sci-Fi</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>Family</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>Fantasy</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Horror</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Musical</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Mystery</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Religious</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Romance</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>Sci-Fi</c:v>
+                  <c:v>Animation</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Thriller</c:v>
+                  <c:v>Adventure</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8902,55 +8914,55 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>233839500</c:v>
+                  <c:v>36914285.714285716</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>308633333.33333331</c:v>
+                  <c:v>53705384.615384616</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>276200000</c:v>
+                  <c:v>57669565.217391305</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>58806666.666666664</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>68500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75646511.627906978</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80990337.078651682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96780000</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>123442857.14285715</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>57669565.217391305</c:v>
+                <c:pt idx="9">
+                  <c:v>130000000</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>68500000</c:v>
+                <c:pt idx="10">
+                  <c:v>136937500</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>80990337.078651682</c:v>
+                <c:pt idx="11">
+                  <c:v>233839500</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
+                  <c:v>244610000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>255443571.42857143</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>270958333.33333331</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>244610000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>75646511.627906978</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>130000000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>96780000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>36914285.714285716</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>53705384.615384616</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>255443571.42857143</c:v>
+                  <c:v>276200000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>136937500</c:v>
+                  <c:v>308633333.33333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9729,15 +9741,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>171449</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17980,7 +17992,7 @@
     <pivotField showAll="0"/>
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="18">
         <item x="1"/>
         <item x="6"/>
@@ -18001,6 +18013,15 @@
         <item x="0"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -18018,55 +18039,55 @@
   </rowFields>
   <rowItems count="18">
     <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
       <x v="13"/>
     </i>
     <i>
       <x v="14"/>
     </i>
     <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
       <x v="15"/>
     </i>
     <i>
-      <x v="16"/>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -18079,7 +18100,7 @@
     <dataField name="Average of Box Office Revenue ($)" fld="13" subtotal="average" baseField="3" baseItem="0" numFmtId="43"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -18406,7 +18427,7 @@
   <dimension ref="A3:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18427,26 +18448,26 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>24</v>
+        <v>871</v>
       </c>
       <c r="B4" s="24">
-        <v>233839500</v>
+        <v>36914285.714285716</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="B5" s="24">
-        <v>308633333.33333331</v>
+        <v>53705384.615384616</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>970</v>
+        <v>33</v>
       </c>
       <c r="B6" s="24">
-        <v>276200000</v>
+        <v>57669565.217391305</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -18459,106 +18480,106 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>42</v>
+        <v>222</v>
       </c>
       <c r="B8" s="24">
-        <v>123442857.14285715</v>
+        <v>68500000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B9" s="24">
-        <v>57669565.217391305</v>
+        <v>75646511.627906978</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>222</v>
+        <v>64</v>
       </c>
       <c r="B10" s="24">
-        <v>68500000</v>
+        <v>80990337.078651682</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>64</v>
+        <v>323</v>
       </c>
       <c r="B11" s="24">
-        <v>80990337.078651682</v>
+        <v>96780000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>191</v>
+        <v>42</v>
       </c>
       <c r="B12" s="24">
-        <v>270958333.33333331</v>
+        <v>123442857.14285715</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>54</v>
+        <v>296</v>
       </c>
       <c r="B13" s="24">
-        <v>244610000</v>
+        <v>130000000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="24">
-        <v>75646511.627906978</v>
+        <v>136937500</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>296</v>
+        <v>24</v>
       </c>
       <c r="B15" s="24">
-        <v>130000000</v>
+        <v>233839500</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>323</v>
+        <v>54</v>
       </c>
       <c r="B16" s="24">
-        <v>96780000</v>
+        <v>244610000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>871</v>
+        <v>159</v>
       </c>
       <c r="B17" s="24">
-        <v>36914285.714285716</v>
+        <v>255443571.42857143</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B18" s="24">
-        <v>53705384.615384616</v>
+        <v>270958333.33333331</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>159</v>
+        <v>970</v>
       </c>
       <c r="B19" s="24">
-        <v>255443571.42857143</v>
+        <v>276200000</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>16</v>
+        <v>145</v>
       </c>
       <c r="B20" s="24">
-        <v>136937500</v>
+        <v>308633333.33333331</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>